<commit_message>
actualizacion de importar preguntas, en el juego la primer respuesta era la correcta, las respuestas se orden de forma RANDOM
</commit_message>
<xml_diff>
--- a/Documentacion/formato preguntas.xlsx
+++ b/Documentacion/formato preguntas.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\Desktop\SETUL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="9135"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,8 +18,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Carvajal Muñoz, Alejandro</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Baja, Media, Alta
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="64">
   <si>
     <t>Pregunta</t>
   </si>
@@ -32,43 +51,201 @@
     <t>Respuesta correcta</t>
   </si>
   <si>
-    <t>Complejidad (baja, media y alta)</t>
-  </si>
-  <si>
-    <t>Las vacaciones a la que todos los trabajadores tienen derecho se deben Pagar en un total de:</t>
-  </si>
-  <si>
-    <t>15 días hábiles</t>
-  </si>
-  <si>
-    <t>20 días hábiles</t>
-  </si>
-  <si>
-    <t>10 días hábiles</t>
-  </si>
-  <si>
-    <t>25 días hábiles</t>
-  </si>
-  <si>
-    <t>baja</t>
-  </si>
-  <si>
     <t>Materia</t>
   </si>
   <si>
     <t>Docente</t>
   </si>
   <si>
-    <t>Respuesta Incorrecta</t>
-  </si>
-  <si>
-    <t>Laboral</t>
+    <t>En un lenguaje débilmente tipado</t>
+  </si>
+  <si>
+    <t>Un valor de un tipo puede ser tratado como de otro tipo siempre que se realice una conversión de forma explícita</t>
+  </si>
+  <si>
+    <t>Un valor de un tipo puede ser tratado como de otro tipo</t>
+  </si>
+  <si>
+    <t>Un valor de un tipo nunca puede ser tratado como de otro tipo</t>
+  </si>
+  <si>
+    <t>Las anteriores respuestas no son correctas</t>
+  </si>
+  <si>
+    <t>Programacion 1</t>
+  </si>
+  <si>
+    <t>Una cola es</t>
+  </si>
+  <si>
+    <t>Una estructura de datos en la que las inserciones se realizan por un extremo y las extracciones por el otro extremo</t>
+  </si>
+  <si>
+    <t>Una estructura de datos en la que las inserciones y extracciones se realizan por el mismo extremo</t>
+  </si>
+  <si>
+    <t>Una estructura de datos en la que sólo se pueden realizar inserciones, pero nunca extracciones</t>
+  </si>
+  <si>
+    <t>Imperativo, declarativo y orientado a objetos son</t>
+  </si>
+  <si>
+    <t>Paradigmas de programación</t>
+  </si>
+  <si>
+    <t>Modos de compilar el código fuente de un programa de ordenador</t>
+  </si>
+  <si>
+    <t>Modos de definir el pseudocódigo de un programa de ordenador</t>
+  </si>
+  <si>
+    <t>Dado el siguiente pseudocódigo, en el que read() permite al usuario introducir un valor entero, ¿cuál será el valor final de la variable "i"?
+i:=1;
+read(n);
+while i &lt; n do begin
+i := i + 1
+end;</t>
+  </si>
+  <si>
+    <t>1 si el valor introducido es igual o menor que 0; el valor introducido menos uno en cualquier otro caso</t>
+  </si>
+  <si>
+    <t>1 si el valor introducido es igual o menor que 1; el valor introducido en cualquier otro caso</t>
+  </si>
+  <si>
+    <t>1 si el valor introducido es igual o menor que 1; el valor introducido más uno en cualquier otro caso</t>
+  </si>
+  <si>
+    <t>if, else, for y while son</t>
+  </si>
+  <si>
+    <t>Sentencias de control</t>
+  </si>
+  <si>
+    <t>Funciones de acceso a datos</t>
+  </si>
+  <si>
+    <t>Tipos de datos</t>
+  </si>
+  <si>
+    <t>Un bucle o ciclo es</t>
+  </si>
+  <si>
+    <t>La programación se puede definir como…</t>
+  </si>
+  <si>
+    <t>Una sentencia que permite ejecutar un bloque aislado de código varias veces hasta que se cumpla (o deje de cumplirse) la condición asignada al bucle</t>
+  </si>
+  <si>
+    <t>Una sentencia que permite decidir si se ejecuta o no se ejecuta una sola vez un bloque aislado de código</t>
+  </si>
+  <si>
+    <t>Una sentencia que ejecuta otra sentencia que a su vez ejecuta la primera sentencia</t>
+  </si>
+  <si>
+    <t>el proceso de diseñar, codificar, depurar y mantener el código fuente de programas de ordenador</t>
+  </si>
+  <si>
+    <t>la ejecución de programas de ordenador desde la línea de comandos</t>
+  </si>
+  <si>
+    <t>la instalación de programas en sistemas operativos desde la línea de comandos</t>
+  </si>
+  <si>
+    <t>El lenguaje ensamblador se sitúa</t>
+  </si>
+  <si>
+    <t>¿Cuál es el código ASCII decimal de "nueva línea" (line feed)?</t>
+  </si>
+  <si>
+    <t>Más cerca del lenguaje máquina que de los lenguajes de alto nivel</t>
+  </si>
+  <si>
+    <t>Más cerca de los lenguajes de alto nivel que del lenguaje máquina</t>
+  </si>
+  <si>
+    <t>No es un lenguaje de programación</t>
+  </si>
+  <si>
+    <t>¿Qué es un algoritmo?</t>
+  </si>
+  <si>
+    <t>Un conjunto de instrucciones o reglas bien definidas, ordenadas y finitas que permiten realizar una actividad mediante pasos sucesivos que no generen dudas a quien deba realizar dicha actividad</t>
+  </si>
+  <si>
+    <t>Es una igualdad entre dos expresiones algebraicas, denominadas miembros, en las que aparecen valores conocidos o datos, y desconocidos o incógnitas, relacionados mediante operaciones</t>
+  </si>
+  <si>
+    <t>Es una relación de variables que pueden ser cuantificadas para calcular el valor de otras de muy difícil o imposible cálculo y que suministra una solución para un problema</t>
+  </si>
+  <si>
+    <t>int, char, float, string y boolean son</t>
+  </si>
+  <si>
+    <t>Instrucciones de acceso a datos</t>
+  </si>
+  <si>
+    <t>¿Qué significa EOF?</t>
+  </si>
+  <si>
+    <t>Se considera que el primer lenguaje de alto nivel fue</t>
+  </si>
+  <si>
+    <t>Empty or full</t>
+  </si>
+  <si>
+    <t>End of file</t>
+  </si>
+  <si>
+    <t>End of floop</t>
+  </si>
+  <si>
+    <t>Fortran</t>
+  </si>
+  <si>
+    <t>Ada</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>El número 1010 en binario se representa en decimal como</t>
+  </si>
+  <si>
+    <t>¿Cuál es el código ASCII decimal de la letra A mayúscula?</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Sistemas</t>
+  </si>
+  <si>
+    <t>Complejidad</t>
+  </si>
+  <si>
+    <t>Respuesta Incorrecta1</t>
+  </si>
+  <si>
+    <t>Respuesta Incorrecta2</t>
+  </si>
+  <si>
+    <t>Respuesta Incorrecta3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,10 +263,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,8 +291,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,78 +567,447 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C10">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
         <v>12</v>
+      </c>
+      <c r="E15">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16">
+        <v>65</v>
+      </c>
+      <c r="C16">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>97</v>
+      </c>
+      <c r="E16">
+        <v>126</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>